<commit_message>
some minor updates after feedback
</commit_message>
<xml_diff>
--- a/Hyperwall_stats.xlsx
+++ b/Hyperwall_stats.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drodriguez/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drodriguez/data/hyperwall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F382C164-774B-DB49-8048-72CCF2F0FCCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3CA5D1-36CF-504B-BC67-4926BC7CB5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1600" windowWidth="28040" windowHeight="17440" xr2:uid="{80839707-F499-4546-A427-4E02420E1512}"/>
+    <workbookView xWindow="4440" yWindow="1600" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{80839707-F499-4546-A427-4E02420E1512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>years</t>
   </si>
@@ -205,17 +205,24 @@
     <t>sum_contentLength</t>
   </si>
   <si>
-    <t>div by 1E9</t>
+    <t>as of Nov 5</t>
+  </si>
+  <si>
+    <t>div by 1024^3</t>
+  </si>
+  <si>
+    <t>3 TB per month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -246,11 +253,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE94B45-3DFE-7547-9C8E-92A5FF91CB8F}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -625,7 +633,7 @@
         <v>1.0506783531158391E-3</v>
       </c>
       <c r="N2" s="3">
-        <f>C2*$B$24</f>
+        <f t="shared" ref="N2:N10" si="0">C2*$B$24</f>
         <v>0.54696057125116415</v>
       </c>
     </row>
@@ -649,11 +657,11 @@
         <v>6.8614594179313607E-2</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J19" si="0">I3/$D$24*100</f>
+        <f t="shared" ref="J3:J19" si="1">I3/$D$24*100</f>
         <v>1.6632646990954975E-4</v>
       </c>
       <c r="N3" s="3">
-        <f>C3*$B$24</f>
+        <f t="shared" si="0"/>
         <v>1.7212045948463209E-2</v>
       </c>
     </row>
@@ -677,11 +685,11 @@
         <v>2.1204885539279901E-3</v>
       </c>
       <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>5.1402093079023251E-6</v>
+      </c>
+      <c r="N4" s="3">
         <f t="shared" si="0"/>
-        <v>5.1402093079023251E-6</v>
-      </c>
-      <c r="N4" s="3">
-        <f>C4*$B$24</f>
         <v>8.6060229742316047E-3</v>
       </c>
     </row>
@@ -705,11 +713,11 @@
         <v>1.7626030036030399E-3</v>
       </c>
       <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>4.2726702525575695E-6</v>
+      </c>
+      <c r="N5" s="3">
         <f t="shared" si="0"/>
-        <v>4.2726702525575695E-6</v>
-      </c>
-      <c r="N5" s="3">
-        <f>C5*$B$24</f>
         <v>7.6497981993169824E-3</v>
       </c>
     </row>
@@ -733,11 +741,11 @@
         <v>9.5768725838168999E-4</v>
       </c>
       <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3214994254386306E-6</v>
+      </c>
+      <c r="N6" s="3">
         <f t="shared" si="0"/>
-        <v>2.3214994254386306E-6</v>
-      </c>
-      <c r="N6" s="3">
-        <f>C6*$B$24</f>
         <v>2.8686743247438684E-3</v>
       </c>
     </row>
@@ -758,11 +766,11 @@
         <v>0.246800793668977</v>
       </c>
       <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>5.9826200639705857E-4</v>
+      </c>
+      <c r="N7" s="3">
         <f t="shared" si="0"/>
-        <v>5.9826200639705857E-4</v>
-      </c>
-      <c r="N7" s="3">
-        <f>C7*$B$24</f>
         <v>4.0161440546414157E-2</v>
       </c>
     </row>
@@ -783,11 +791,11 @@
         <v>0.130389167940822</v>
       </c>
       <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1607226243099689E-4</v>
+      </c>
+      <c r="N8" s="3">
         <f t="shared" si="0"/>
-        <v>3.1607226243099689E-4</v>
-      </c>
-      <c r="N8" s="3">
-        <f>C8*$B$24</f>
         <v>0.12430922073890097</v>
       </c>
     </row>
@@ -808,11 +816,11 @@
         <v>9</v>
       </c>
       <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
-        <f>C9*$B$24</f>
         <v>77</v>
       </c>
     </row>
@@ -836,11 +844,11 @@
         <v>122.94196580725099</v>
       </c>
       <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.29801973502928014</v>
+      </c>
+      <c r="N10" s="3">
         <f t="shared" si="0"/>
-        <v>0.29801973502928014</v>
-      </c>
-      <c r="N10" s="3">
-        <f>C10*$B$24</f>
         <v>0.34328469419434954</v>
       </c>
     </row>
@@ -855,7 +863,7 @@
         <v>12</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11" s="3"/>
@@ -877,11 +885,11 @@
         <v>40</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <f>C12*$B$24</f>
+        <f t="shared" ref="N12:N19" si="2">C12*$B$24</f>
         <v>2.4135113318845081</v>
       </c>
     </row>
@@ -899,11 +907,11 @@
         <v>14</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13" s="3">
-        <f>C13*$B$24</f>
+        <f t="shared" si="2"/>
         <v>11.374293697609437</v>
       </c>
     </row>
@@ -921,11 +929,11 @@
         <v>15</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14" s="3">
-        <f>C14*$B$24</f>
+        <f t="shared" si="2"/>
         <v>73.16936355169203</v>
       </c>
     </row>
@@ -940,11 +948,11 @@
         <v>17.190000000000001</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N15" s="3">
-        <f>C15*$B$24</f>
+        <f t="shared" si="2"/>
         <v>16.437503880782366</v>
       </c>
     </row>
@@ -959,11 +967,11 @@
         <v>14.497999999999999</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N16" s="3">
-        <f>C16*$B$24</f>
+        <f t="shared" si="2"/>
         <v>13.863346786712201</v>
       </c>
     </row>
@@ -981,11 +989,11 @@
         <v>17</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N17" s="3">
-        <f>C17*$B$24</f>
+        <f t="shared" si="2"/>
         <v>91.013474076373797</v>
       </c>
     </row>
@@ -1003,11 +1011,11 @@
         <v>18</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N18" s="3">
-        <f>C18*$B$24</f>
+        <f t="shared" si="2"/>
         <v>81.843278484942559</v>
       </c>
     </row>
@@ -1029,11 +1037,11 @@
         <v>7.3455372995226323E-2</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7806084889544828E-4</v>
       </c>
       <c r="N19" s="3">
-        <f>C19*$B$24</f>
+        <f t="shared" si="2"/>
         <v>2.5818068922694816E-2</v>
       </c>
     </row>
@@ -1074,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16235387-2054-2543-91D5-9B957548F840}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,7 +1105,7 @@
         <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1178,9 +1186,9 @@
       <c r="D10">
         <v>781273638008</v>
       </c>
-      <c r="E10">
-        <f>D10/1000000000</f>
-        <v>781.27363800800003</v>
+      <c r="E10" s="4">
+        <f>D10/(1024*1024*1024)</f>
+        <v>727.61777602881193</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,7 +1243,7 @@
         <v>22028142</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1243,7 +1251,7 @@
         <v>117608</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1251,15 +1259,28 @@
         <v>266243</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
       <c r="B19">
         <v>73664</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>34821786831339</v>
+      </c>
+      <c r="E19" s="4">
+        <f>D19/(1024*1024*1024)</f>
+        <v>32430.316164474003</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1267,7 +1288,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1275,7 +1296,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23">
         <f>SUM(B2:B21)</f>
         <v>30036470</v>

</xml_diff>

<commit_message>
new version of coverage figures
</commit_message>
<xml_diff>
--- a/Hyperwall_stats.xlsx
+++ b/Hyperwall_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drodriguez/data/hyperwall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3CA5D1-36CF-504B-BC67-4926BC7CB5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF5CF07-156A-2645-AC10-3E1D6BA45747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1600" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{80839707-F499-4546-A427-4E02420E1512}"/>
+    <workbookView xWindow="2500" yWindow="6420" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{80839707-F499-4546-A427-4E02420E1512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>years</t>
   </si>
@@ -208,23 +208,51 @@
     <t>as of Nov 5</t>
   </si>
   <si>
-    <t>div by 1024^3</t>
-  </si>
-  <si>
     <t>3 TB per month</t>
+  </si>
+  <si>
+    <t>from SR15 (GB)</t>
+  </si>
+  <si>
+    <t>in GB</t>
+  </si>
+  <si>
+    <t>1024^3</t>
+  </si>
+  <si>
+    <t>1 billion</t>
+  </si>
+  <si>
+    <t>num_files</t>
+  </si>
+  <si>
+    <t>totals</t>
+  </si>
+  <si>
+    <t>shuttle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,17 +278,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -576,7 +613,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,165 +1119,329 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16235387-2054-2543-91D5-9B957548F840}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
       </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
       <c r="D1" t="s">
         <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2">
         <v>319</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>2725</v>
+      </c>
+      <c r="D2">
+        <v>2451198076</v>
+      </c>
+      <c r="E2" s="7">
+        <f>D2/$E$24</f>
+        <v>2.2828561030328274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
         <v>1367</v>
       </c>
-      <c r="G3">
-        <f>SUM(B2,B9,B20:B21)</f>
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>9842</v>
+      </c>
+      <c r="D3">
+        <v>81583137856</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E21" si="0">D3/$E$24</f>
+        <v>75.98021799325943</v>
+      </c>
+      <c r="H3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4">
         <v>5731</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1532075</v>
+      </c>
+      <c r="D4">
+        <v>587677729967</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>547.31753651704639</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5">
         <v>274911</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>18840050</v>
+      </c>
+      <c r="D5" s="6">
+        <v>17990760357811</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>16755.201255726628</v>
+      </c>
+      <c r="H5" s="4">
+        <v>28590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
       <c r="B6">
         <v>900019</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>2248346</v>
+      </c>
+      <c r="D6" s="6">
+        <v>57908050171200</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>53931.074376404285</v>
+      </c>
+      <c r="H6" s="4">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7">
         <v>3169946</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>9406271</v>
+      </c>
+      <c r="D7" s="6">
+        <v>9379144910661</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>8735.0093858884647</v>
+      </c>
+      <c r="H7" s="4">
+        <v>7505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
       <c r="B8">
         <v>1357515</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>17422033</v>
+      </c>
+      <c r="D8" s="6">
+        <v>146618669070408</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>136549.27636534721</v>
+      </c>
+      <c r="H8" s="4">
+        <v>107230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9">
         <v>653</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>8726</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3143178514</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>2.9273131061345339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10">
         <v>101971</v>
       </c>
-      <c r="D10">
-        <v>781273638008</v>
-      </c>
-      <c r="E10" s="4">
-        <f>D10/(1024*1024*1024)</f>
-        <v>727.61777602881193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>955434</v>
+      </c>
+      <c r="D10" s="6">
+        <v>191035141255</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>177.91533959563822</v>
+      </c>
+      <c r="H10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11">
         <v>27550</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="6"/>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12">
         <v>1492746</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>3342905</v>
+      </c>
+      <c r="D12" s="6">
+        <v>4403495417547</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>4101.0746895773336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>50</v>
       </c>
       <c r="B13">
         <v>532</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>1596</v>
+      </c>
+      <c r="D13" s="6">
+        <v>216871527936</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>201.97734975814819</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14">
         <v>212993</v>
+      </c>
+      <c r="C14">
+        <v>6728700</v>
+      </c>
+      <c r="D14" s="6">
+        <v>17350990159044</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>16159.368827048689</v>
       </c>
       <c r="G14">
         <f>SUM(B14:B15)</f>
         <v>217129</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
       <c r="B15">
         <v>4136</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>12408</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1687020315648</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>1571.1601037979126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16">
         <v>22028142</v>
+      </c>
+      <c r="C16">
+        <v>104280276</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1177090480293440</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>1096250.9366622567</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1250,6 +1451,11 @@
       <c r="B17">
         <v>117608</v>
       </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1258,6 +1464,19 @@
       <c r="B18">
         <v>266243</v>
       </c>
+      <c r="C18">
+        <v>1407298</v>
+      </c>
+      <c r="D18" s="6">
+        <v>7621203911483</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>7097.799248511903</v>
+      </c>
+      <c r="H18">
+        <v>6641</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1266,18 +1485,21 @@
       <c r="B19">
         <v>73664</v>
       </c>
-      <c r="D19">
+      <c r="C19">
+        <v>1353640</v>
+      </c>
+      <c r="D19" s="6">
         <v>34821786831339</v>
       </c>
-      <c r="E19" s="4">
-        <f>D19/(1024*1024*1024)</f>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
         <v>32430.316164474003</v>
       </c>
       <c r="F19" t="s">
         <v>57</v>
       </c>
       <c r="I19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1287,6 +1509,16 @@
       <c r="B20">
         <v>186</v>
       </c>
+      <c r="C20">
+        <v>4678</v>
+      </c>
+      <c r="D20" s="6">
+        <v>218829672</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="0"/>
+        <v>0.20380101352930069</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1295,11 +1527,65 @@
       <c r="B21">
         <v>238</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B23">
+      <c r="C21">
+        <v>1429</v>
+      </c>
+      <c r="D21" s="6">
+        <v>15079956</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="0"/>
+        <v>1.4044303447008133E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24">
+        <f>1024*1024*1024</f>
+        <v>1073741824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <f>SUM(B2,B9,B20:B21)</f>
+        <v>1396</v>
+      </c>
+      <c r="H27" s="10">
+        <f>E2+E9+E20+E21</f>
+        <v>5.4280145261436701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="8">
         <f>SUM(B2:B21)</f>
         <v>30036470</v>
+      </c>
+      <c r="C28" s="8">
+        <f>SUM(C2:C21)</f>
+        <v>167558432</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8">
+        <f>SUM(E2:E21)</f>
+        <v>1374589.8355374234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating versions and text
</commit_message>
<xml_diff>
--- a/Hyperwall_stats.xlsx
+++ b/Hyperwall_stats.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drodriguez/data/hyperwall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2448D33D-FA8C-FF40-9C40-67203D4B0EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D89BD3-1D0F-6648-8E2D-029EBBFF5BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="6400" windowWidth="28040" windowHeight="17440" xr2:uid="{80839707-F499-4546-A427-4E02420E1512}"/>
+    <workbookView xWindow="8120" yWindow="3920" windowWidth="31200" windowHeight="20920" activeTab="2" xr2:uid="{80839707-F499-4546-A427-4E02420E1512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet3!$A$3:$A$9</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet3!$B$3:$B$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>years</t>
   </si>
@@ -236,6 +241,12 @@
   </si>
   <si>
     <t>2010-2014</t>
+  </si>
+  <si>
+    <t>Smaller Missions</t>
+  </si>
+  <si>
+    <t>Kepler &amp; K2</t>
   </si>
 </sst>
 </file>
@@ -308,6 +319,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB391B5"/>
+      <color rgb="FFFF8F7F"/>
+      <color rgb="FFFFDF71"/>
+      <color rgb="FF5ABBA7"/>
+      <color rgb="FFA3D977"/>
+      <color rgb="FFFFC374"/>
+      <color rgb="FF99D2F3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -317,6 +339,1214 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="99D2F3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC374"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="5ABBA7"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFDF71"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF8F7F"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="A3D977"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="B391B5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-074F-654C-B20B-F0C6856E397D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0697114327189547E-2"/>
+                  <c:y val="0.1957855196398729"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-074F-654C-B20B-F0C6856E397D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8616878546606153E-2"/>
+                  <c:y val="-0.12706945092666477"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-074F-654C-B20B-F0C6856E397D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8228016539831962E-2"/>
+                  <c:y val="-3.6741090920040347E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-074F-654C-B20B-F0C6856E397D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.3635353890819515E-2"/>
+                  <c:y val="1.6075789283509733E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-074F-654C-B20B-F0C6856E397D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3798882681565268E-3"/>
+                  <c:y val="2.4494662832537904E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-074F-654C-B20B-F0C6856E397D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>GALEX</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>HST</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HLSP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>IUE</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SWIFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>TESS</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Kepler &amp; K2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PS1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$3:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>274911</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2257534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3169946</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101971</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>266243</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>658116</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1710407</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22028142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-074F-654C-B20B-F0C6856E397D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B29BC4-5AEA-0045-9862-C695BF60C311}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -618,7 +1848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE94B45-3DFE-7547-9C8E-92A5FF91CB8F}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -672,11 +1902,11 @@
         <v>0.43343593386691398</v>
       </c>
       <c r="J2" s="1">
-        <f>I2/$D$25*100</f>
+        <f t="shared" ref="J2:J15" si="0">I2/$D$25*100</f>
         <v>1.0506783531158391E-3</v>
       </c>
       <c r="N2" s="3">
-        <f>C2*$B$25</f>
+        <f t="shared" ref="N2:N13" si="1">C2*$B$25</f>
         <v>0.54696057125116415</v>
       </c>
     </row>
@@ -700,11 +1930,11 @@
         <v>6.8614594179313607E-2</v>
       </c>
       <c r="J3" s="1">
-        <f>I3/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>1.6632646990954975E-4</v>
       </c>
       <c r="N3" s="3">
-        <f>C3*$B$25</f>
+        <f t="shared" si="1"/>
         <v>1.7212045948463209E-2</v>
       </c>
     </row>
@@ -728,11 +1958,11 @@
         <v>2.1204885539279901E-3</v>
       </c>
       <c r="J4" s="1">
-        <f>I4/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>5.1402093079023251E-6</v>
       </c>
       <c r="N4" s="3">
-        <f>C4*$B$25</f>
+        <f t="shared" si="1"/>
         <v>8.6060229742316047E-3</v>
       </c>
     </row>
@@ -756,11 +1986,11 @@
         <v>1.7626030036030399E-3</v>
       </c>
       <c r="J5" s="1">
-        <f>I5/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>4.2726702525575695E-6</v>
       </c>
       <c r="N5" s="3">
-        <f>C5*$B$25</f>
+        <f t="shared" si="1"/>
         <v>7.6497981993169824E-3</v>
       </c>
     </row>
@@ -784,11 +2014,11 @@
         <v>9.5768725838168999E-4</v>
       </c>
       <c r="J6" s="1">
-        <f>I6/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>2.3214994254386306E-6</v>
       </c>
       <c r="N6" s="3">
-        <f>C6*$B$25</f>
+        <f t="shared" si="1"/>
         <v>2.8686743247438684E-3</v>
       </c>
     </row>
@@ -809,11 +2039,11 @@
         <v>0.246800793668977</v>
       </c>
       <c r="J7" s="1">
-        <f>I7/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>5.9826200639705857E-4</v>
       </c>
       <c r="N7" s="3">
-        <f>C7*$B$25</f>
+        <f t="shared" si="1"/>
         <v>4.0161440546414157E-2</v>
       </c>
     </row>
@@ -834,11 +2064,11 @@
         <v>40</v>
       </c>
       <c r="J8" s="1">
-        <f>I8/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N8" s="3">
-        <f>C8*$B$25</f>
+        <f t="shared" si="1"/>
         <v>2.4135113318845081</v>
       </c>
     </row>
@@ -859,11 +2089,11 @@
         <v>0.130389167940822</v>
       </c>
       <c r="J9" s="1">
-        <f>I9/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>3.1607226243099689E-4</v>
       </c>
       <c r="N9" s="3">
-        <f>C9*$B$25</f>
+        <f t="shared" si="1"/>
         <v>0.12430922073890097</v>
       </c>
     </row>
@@ -884,11 +2114,11 @@
         <v>9</v>
       </c>
       <c r="J10" s="1">
-        <f>I10/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" s="3">
-        <f>C10*$B$25</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
@@ -906,11 +2136,11 @@
         <v>14</v>
       </c>
       <c r="J11" s="1">
-        <f>I11/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N11" s="3">
-        <f>C11*$B$25</f>
+        <f t="shared" si="1"/>
         <v>11.374293697609437</v>
       </c>
     </row>
@@ -934,11 +2164,11 @@
         <v>122.94196580725099</v>
       </c>
       <c r="J12" s="1">
-        <f>I12/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0.29801973502928014</v>
       </c>
       <c r="N12" s="3">
-        <f>C12*$B$25</f>
+        <f t="shared" si="1"/>
         <v>0.34328469419434954</v>
       </c>
     </row>
@@ -959,11 +2189,11 @@
         <v>15</v>
       </c>
       <c r="J13" s="1">
-        <f>I13/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" s="3">
-        <f>C13*$B$25</f>
+        <f t="shared" si="1"/>
         <v>73.16936355169203</v>
       </c>
     </row>
@@ -978,7 +2208,7 @@
         <v>12</v>
       </c>
       <c r="J14" s="1">
-        <f>I14/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14" s="3"/>
@@ -994,7 +2224,7 @@
         <v>17.190000000000001</v>
       </c>
       <c r="J15" s="1">
-        <f>I15/$D$25*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15" s="3">
@@ -1141,13 +2371,13 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A21" sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
@@ -1611,4 +2841,300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C15220-8E4C-984D-8EB2-28D8EB0271BC}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <f>SUM(B18:B20)</f>
+        <v>8494</v>
+      </c>
+      <c r="C2">
+        <f>SUM(C18:C20)</f>
+        <v>1559475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>274911</v>
+      </c>
+      <c r="C3">
+        <v>18840050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B29:B30)</f>
+        <v>2257534</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C29:C30)</f>
+        <v>19670379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>3169946</v>
+      </c>
+      <c r="C5">
+        <v>9406271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>101971</v>
+      </c>
+      <c r="C6">
+        <v>955434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>266243</v>
+      </c>
+      <c r="C7">
+        <v>1407298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>658116</v>
+      </c>
+      <c r="C8">
+        <v>1433609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B22:B25)</f>
+        <v>1710407</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C22:C25)</f>
+        <v>10085609</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>22028142</v>
+      </c>
+      <c r="C10">
+        <v>104280276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>653</v>
+      </c>
+      <c r="C13">
+        <v>8726</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>319</v>
+      </c>
+      <c r="C14">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>186</v>
+      </c>
+      <c r="C15">
+        <v>4678</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>238</v>
+      </c>
+      <c r="C16">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B13:B16)</f>
+        <v>1396</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C13:C16)</f>
+        <v>17558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>1367</v>
+      </c>
+      <c r="C19">
+        <v>9842</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>5731</v>
+      </c>
+      <c r="C20">
+        <v>1532075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>1492746</v>
+      </c>
+      <c r="C22">
+        <v>3342905</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>532</v>
+      </c>
+      <c r="C23">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>212993</v>
+      </c>
+      <c r="C24">
+        <v>6728700</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25">
+        <v>4136</v>
+      </c>
+      <c r="C25">
+        <v>12408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>117608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29">
+        <v>900019</v>
+      </c>
+      <c r="C29">
+        <v>2248346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>1357515</v>
+      </c>
+      <c r="C30">
+        <v>17422033</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32">
+        <v>27550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>